<commit_message>
convert decimal value to integer
</commit_message>
<xml_diff>
--- a/automate-excel-tasks/project-migrating-text-to-excel/MyCompanyStaff.xlsx
+++ b/automate-excel-tasks/project-migrating-text-to-excel/MyCompanyStaff.xlsx
@@ -481,10 +481,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -501,27 +499,21 @@
           <t>Sales</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>121921900</t>
-        </is>
+      <c r="E2" t="n">
+        <v>121921900</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>1st Address, Miami</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>52000</t>
-        </is>
+      <c r="G2" t="n">
+        <v>52000</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -538,27 +530,21 @@
           <t>IT</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>12918210</t>
-        </is>
+      <c r="E3" t="n">
+        <v>12918210</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
           <t>2nd Address, Miami</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>52200</t>
-        </is>
+      <c r="G3" t="n">
+        <v>52200</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -575,27 +561,21 @@
           <t>IT</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>20192101</t>
-        </is>
+      <c r="E4" t="n">
+        <v>20192101</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>3rd Address, Miami</t>
         </is>
       </c>
-      <c r="G4" s="1" t="inlineStr">
-        <is>
-          <t>58000</t>
-        </is>
+      <c r="G4" s="1" t="n">
+        <v>58000</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -612,27 +592,21 @@
           <t>Marketing</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>31312311</t>
-        </is>
+      <c r="E5" t="n">
+        <v>31312311</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>4th Address, Miami</t>
         </is>
       </c>
-      <c r="G5" s="1" t="inlineStr">
-        <is>
-          <t>58700</t>
-        </is>
+      <c r="G5" s="1" t="n">
+        <v>58700</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -649,27 +623,21 @@
           <t>Marketing</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>43423434</t>
-        </is>
+      <c r="E6" t="n">
+        <v>43423434</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>5th Address, Miami</t>
         </is>
       </c>
-      <c r="G6" s="1" t="inlineStr">
-        <is>
-          <t>60000</t>
-        </is>
+      <c r="G6" s="1" t="n">
+        <v>60000</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -686,27 +654,21 @@
           <t>Sales</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>323232291</t>
-        </is>
+      <c r="E7" t="n">
+        <v>323232291</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>6th Address, Miami</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>54000</t>
-        </is>
+      <c r="G7" t="n">
+        <v>54000</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -723,27 +685,21 @@
           <t>Logistics</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>1277177910</t>
-        </is>
+      <c r="E8" t="n">
+        <v>1277177910</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>7th Address, Miami</t>
         </is>
       </c>
-      <c r="G8" s="1" t="inlineStr">
-        <is>
-          <t>56000</t>
-        </is>
+      <c r="G8" s="1" t="n">
+        <v>56000</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -760,27 +716,21 @@
           <t>Sales</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>3691919186</t>
-        </is>
+      <c r="E9" t="n">
+        <v>3691919186</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
           <t>8th Address, Miami</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>49000</t>
-        </is>
+      <c r="G9" t="n">
+        <v>49000</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -797,27 +747,21 @@
           <t>IT</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>215557299</t>
-        </is>
+      <c r="E10" t="n">
+        <v>215557299</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
           <t>9th Address, Miami</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>53000</t>
-        </is>
+      <c r="G10" t="n">
+        <v>53000</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="A11" t="n">
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -834,20 +778,16 @@
           <t>Logistics</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>3266617791</t>
-        </is>
+      <c r="E11" t="n">
+        <v>3266617791</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>10th Address, Miami</t>
         </is>
       </c>
-      <c r="G11" s="1" t="inlineStr">
-        <is>
-          <t>59500</t>
-        </is>
+      <c r="G11" s="1" t="n">
+        <v>59500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>